<commit_message>
Updated code with new changes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,9 +586,310 @@
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Submission Date</t>
-        </is>
-      </c>
+          <t>Today  Date</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Today Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DHARMANA DHANA LAKSHMI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dhana</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Laxman</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Tulasi</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>9493541829</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dharmanadhanalaxmi006@outlook.com</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Andhra Pradesh state, Srikakulam district.</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>463426316719</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>9550791829</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2025-04-16</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Full-Time</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Ganesh</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>1253647890</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Dhana Lakshmi</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>XXXXXXXXX10</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Canva</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Headset</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Dhana Lakshmi</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tejaswnini</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Teju</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ramana</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sita</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7675993724</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>tejaswanipulugu171@gmail.com</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>amalapuram</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>123456789123</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Dhana</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>9493541829</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2025-04-16</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Full-Time</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>John Kiran</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Office</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>1253647890</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Dhana Lakshmi</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>XXXXXXXXX10</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Canva</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Headset</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Tejaswini</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>